<commit_message>
back validación existencia de insumos
</commit_message>
<xml_diff>
--- a/repon/administracion/static/formatoValidaciones.xlsx
+++ b/repon/administracion/static/formatoValidaciones.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juanyepes\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juanyepes\Desktop\proyectoP2v1\capsule\proyecto\repon\administracion\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{66D2B493-EB7C-4545-B462-DED78EB61105}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F5D7430-7B76-4A76-8644-B73F1DEDAF18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{2580DE46-E291-421F-B393-36EB422C84BF}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{2580DE46-E291-421F-B393-36EB422C84BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Codigo_insumo</t>
   </si>
@@ -48,13 +48,37 @@
   </si>
   <si>
     <t>Cantidad</t>
+  </si>
+  <si>
+    <t>Teja</t>
+  </si>
+  <si>
+    <t>Und</t>
+  </si>
+  <si>
+    <t>20.0</t>
+  </si>
+  <si>
+    <t>Tubo pvc 1/4</t>
+  </si>
+  <si>
+    <t>Mts</t>
+  </si>
+  <si>
+    <t>40.0</t>
+  </si>
+  <si>
+    <t>Arena de construcción</t>
+  </si>
+  <si>
+    <t>Kg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -62,16 +86,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="MS Shell Dlg 2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -79,15 +122,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,20 +467,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACB871BA-AD25-41B7-B99D-CB2AFF6D4623}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -428,6 +493,49 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>20193</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>29461</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>234654</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4">
+        <v>30</v>
+      </c>
+      <c r="E4" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>